<commit_message>
Printing complex types, properties in complex types. Missing formatting and proper index handling
</commit_message>
<xml_diff>
--- a/Assets/Template.xlsx
+++ b/Assets/Template.xlsx
@@ -58,7 +58,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,14 +78,6 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -133,9 +125,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
   </cellXfs>
@@ -422,9 +413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="XFD11" sqref="XFD11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -433,40 +422,40 @@
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="4" max="4" width="47.5703125" customWidth="1"/>
     <col min="5" max="16383" width="9.140625" hidden="1"/>
-    <col min="16384" max="16384" width="32.28515625" customWidth="1"/>
+    <col min="16384" max="16384" width="32.28515625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -484,11 +473,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>